<commit_message>
Commit standing frame BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/GitHub/unitree-qmini-robot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/GitHub/Unitree-Qmini-Robot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A98B84-3508-2A4C-841B-96177CC6210A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B60B166-980A-7840-92C7-CD83E6185DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="500" windowWidth="45800" windowHeight="27260" activeTab="1" xr2:uid="{AB9389B4-2FA2-4848-9210-F8543C78B964}"/>
+    <workbookView xWindow="4440" yWindow="500" windowWidth="45820" windowHeight="38620" activeTab="1" xr2:uid="{AB9389B4-2FA2-4848-9210-F8543C78B964}"/>
   </bookViews>
   <sheets>
     <sheet name="3D Print" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="180">
   <si>
     <t>Right Foot A</t>
   </si>
@@ -559,6 +559,24 @@
   </si>
   <si>
     <t>2档</t>
+  </si>
+  <si>
+    <t>https://www.misumi.com.cn/vona2/detail/110310158399/?ProductCode=LCFB6-2040-200-TPW</t>
+  </si>
+  <si>
+    <t>站立调试底座</t>
+  </si>
+  <si>
+    <t>2040 型材</t>
+  </si>
+  <si>
+    <t>经济型欧标槽宽 6mm</t>
+  </si>
+  <si>
+    <t>M3.5 x 16</t>
+  </si>
+  <si>
+    <t>上身电机上盖底部限位</t>
   </si>
 </sst>
 </file>
@@ -2072,17 +2090,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33821E08-F46F-4446-B9C0-A0B043389FFA}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" style="2" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="64.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="36" customWidth="1"/>
@@ -2192,7 +2210,7 @@
         <v>0.2</v>
       </c>
       <c r="G5" s="43">
-        <f t="shared" ref="G5:G40" si="0">E5*F5</f>
+        <f t="shared" ref="G5:G41" si="0">E5*F5</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -2508,26 +2526,24 @@
     </row>
     <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>115</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="C19" s="41"/>
       <c r="D19" s="10" t="s">
-        <v>22</v>
+        <v>179</v>
       </c>
       <c r="E19" s="12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F19" s="40">
-        <v>1.0620000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="G19" s="43">
         <f t="shared" si="0"/>
-        <v>2.1240000000000001</v>
+        <v>1.7999999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2535,34 +2551,34 @@
         <v>112</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="E20" s="12">
         <v>2</v>
       </c>
       <c r="F20" s="40">
-        <v>1.585</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="G20" s="43">
-        <f t="shared" ref="G20" si="4">E20*F20</f>
-        <v>3.17</v>
+        <f t="shared" si="0"/>
+        <v>2.1240000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>143</v>
@@ -2571,260 +2587,260 @@
         <v>2</v>
       </c>
       <c r="F21" s="40">
-        <v>0.46</v>
+        <v>1.585</v>
       </c>
       <c r="G21" s="43">
-        <f t="shared" ref="G21" si="5">E21*F21</f>
-        <v>0.92</v>
+        <f t="shared" ref="G21" si="4">E21*F21</f>
+        <v>3.17</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="40">
+        <v>0.46</v>
+      </c>
+      <c r="G22" s="43">
+        <f t="shared" ref="G22" si="5">E22*F22</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C23" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E23" s="12">
         <v>1</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F23" s="40">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G23" s="43">
         <f t="shared" si="0"/>
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="24" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C24" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="12">
+      <c r="D24" s="10"/>
+      <c r="E24" s="12">
         <v>2</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F24" s="40">
         <v>8</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G24" s="43">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="25" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C25" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="12">
+      <c r="D25" s="10"/>
+      <c r="E25" s="12">
         <v>1</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F25" s="40">
         <v>199</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G25" s="43">
         <f t="shared" si="0"/>
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="12">
-        <v>5</v>
-      </c>
-      <c r="F25" s="40">
-        <v>897</v>
-      </c>
-      <c r="G25" s="43">
-        <f>E25*F25</f>
-        <v>4485</v>
-      </c>
-    </row>
     <row r="26" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>163</v>
+        <v>84</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26" s="40">
-        <v>49</v>
+        <v>897</v>
       </c>
       <c r="G26" s="43">
-        <f t="shared" ref="G26" si="6">E26*F26</f>
-        <v>196</v>
+        <f>E26*F26</f>
+        <v>4485</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F27" s="40">
-        <v>377</v>
+        <v>49</v>
       </c>
       <c r="G27" s="43">
-        <f>E27*F27</f>
-        <v>377</v>
+        <f t="shared" ref="G27" si="6">E27*F27</f>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="12">
         <v>1</v>
       </c>
       <c r="F28" s="40">
-        <v>1999</v>
+        <v>377</v>
       </c>
       <c r="G28" s="43">
         <f>E28*F28</f>
-        <v>1999</v>
+        <v>377</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="12">
         <v>1</v>
       </c>
       <c r="F29" s="40">
-        <v>600</v>
+        <v>1999</v>
       </c>
       <c r="G29" s="43">
         <f>E29*F29</f>
-        <v>600</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="12">
         <v>1</v>
       </c>
       <c r="F30" s="40">
-        <v>265</v>
+        <v>600</v>
       </c>
       <c r="G30" s="43">
         <f>E30*F30</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="12">
+        <v>1</v>
+      </c>
+      <c r="F31" s="40">
         <v>265</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="50" t="s">
+      <c r="G31" s="43">
+        <f>E31*F31</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="52"/>
-    </row>
-    <row r="32" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="12">
-        <v>50</v>
-      </c>
-      <c r="F32" s="40">
-        <v>0.3</v>
-      </c>
-      <c r="G32" s="43">
-        <f t="shared" ref="G32:G36" si="7">E32*F32</f>
-        <v>15</v>
-      </c>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
     </row>
     <row r="33" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E33" s="12">
         <v>50</v>
@@ -2833,300 +2849,300 @@
         <v>0.3</v>
       </c>
       <c r="G33" s="43">
-        <f t="shared" ref="G33" si="8">E33*F33</f>
+        <f t="shared" ref="G33:G37" si="7">E33*F33</f>
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="12">
+        <v>50</v>
+      </c>
+      <c r="F34" s="40">
+        <v>0.3</v>
+      </c>
+      <c r="G34" s="43">
+        <f t="shared" ref="G34" si="8">E34*F34</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B35" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C35" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E35" s="12">
         <v>12</v>
       </c>
-      <c r="F34" s="40">
+      <c r="F35" s="40">
         <v>0.36</v>
       </c>
-      <c r="G34" s="43">
+      <c r="G35" s="43">
         <f t="shared" si="7"/>
         <v>4.32</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="12">
-        <v>4</v>
-      </c>
-      <c r="F35" s="40">
-        <v>16.5</v>
-      </c>
-      <c r="G35" s="43">
-        <f t="shared" si="7"/>
-        <v>66</v>
-      </c>
-    </row>
     <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="12">
         <v>4</v>
       </c>
       <c r="F36" s="40">
-        <v>897</v>
+        <v>16.5</v>
       </c>
       <c r="G36" s="43">
         <f t="shared" si="7"/>
-        <v>3588</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>163</v>
+        <v>84</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="12">
         <v>4</v>
       </c>
       <c r="F37" s="40">
+        <v>897</v>
+      </c>
+      <c r="G37" s="43">
+        <f t="shared" si="7"/>
+        <v>3588</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="12">
+        <v>4</v>
+      </c>
+      <c r="F38" s="40">
         <v>49</v>
       </c>
-      <c r="G37" s="43">
+      <c r="G38" s="43">
         <f t="shared" si="0"/>
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="50" t="s">
+    <row r="39" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="51"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="52"/>
-    </row>
-    <row r="39" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52"/>
+    </row>
+    <row r="40" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C40" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E40" s="12">
         <v>6</v>
       </c>
-      <c r="F39" s="40">
+      <c r="F40" s="40">
         <v>0.2</v>
       </c>
-      <c r="G39" s="43">
+      <c r="G40" s="43">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
+    <row r="41" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B41" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C41" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="12">
+      <c r="D41" s="10"/>
+      <c r="E41" s="12">
         <v>6</v>
       </c>
-      <c r="F40" s="40">
+      <c r="F41" s="40">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G40" s="43">
+      <c r="G41" s="43">
         <f t="shared" si="0"/>
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="12">
-        <v>12</v>
-      </c>
-      <c r="F41" s="40">
-        <v>0.3</v>
-      </c>
-      <c r="G41" s="43">
-        <f t="shared" ref="G41" si="9">E41*F41</f>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
     <row r="42" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
+        <v>87</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>91</v>
+      </c>
       <c r="D42" s="10"/>
       <c r="E42" s="12">
+        <v>12</v>
+      </c>
+      <c r="F42" s="40">
+        <v>0.3</v>
+      </c>
+      <c r="G42" s="43">
+        <f t="shared" ref="G42" si="9">E42*F42</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="12">
         <v>2</v>
       </c>
-      <c r="F42" s="40">
+      <c r="F43" s="40">
         <v>100</v>
-      </c>
-      <c r="G42" s="43">
-        <f>E42*F42</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" s="46"/>
-      <c r="E43" s="48">
-        <v>2</v>
-      </c>
-      <c r="F43" s="49">
-        <v>897</v>
       </c>
       <c r="G43" s="43">
         <f>E43*F43</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="46"/>
+      <c r="E44" s="48">
+        <v>2</v>
+      </c>
+      <c r="F44" s="49">
+        <v>897</v>
+      </c>
+      <c r="G44" s="43">
+        <f>E44*F44</f>
         <v>1794</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="50" t="s">
+    <row r="45" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="52"/>
-    </row>
-    <row r="45" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="12">
-        <v>2</v>
-      </c>
-      <c r="F45" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="G45" s="43">
-        <f>E45*F45</f>
-        <v>0.4</v>
-      </c>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="52"/>
     </row>
     <row r="46" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="E46" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F46" s="40">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G46" s="43">
-        <f t="shared" ref="G46" si="10">E46*F46</f>
-        <v>1.2</v>
+        <f>E46*F46</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E47" s="12">
         <v>4</v>
       </c>
       <c r="F47" s="40">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="G47" s="43">
-        <f t="shared" ref="G47" si="11">E47*F47</f>
-        <v>1.1200000000000001</v>
+        <f t="shared" ref="G47" si="10">E47*F47</f>
+        <v>1.2</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3134,76 +3150,100 @@
         <v>92</v>
       </c>
       <c r="B48" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" s="12">
+        <v>4</v>
+      </c>
+      <c r="F48" s="40">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G48" s="43">
+        <f t="shared" ref="G48" si="11">E48*F48</f>
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="41" t="s">
+      <c r="C49" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E49" s="12">
         <v>2</v>
       </c>
-      <c r="F48" s="40">
+      <c r="F49" s="40">
         <v>0.21</v>
       </c>
-      <c r="G48" s="43">
-        <f t="shared" ref="G48" si="12">E48*F48</f>
+      <c r="G49" s="43">
+        <f t="shared" ref="G49" si="12">E49*F49</f>
         <v>0.42</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="50" t="s">
+    <row r="50" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="52"/>
-    </row>
-    <row r="50" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="52"/>
+    </row>
+    <row r="51" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="12">
-        <v>1</v>
-      </c>
-      <c r="F50" s="40">
-        <v>5</v>
-      </c>
-      <c r="G50" s="43">
-        <f t="shared" ref="G50:G57" si="13">E50*F50</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="40"/>
+      <c r="E51" s="12">
+        <v>1</v>
+      </c>
+      <c r="F51" s="40">
+        <v>5</v>
+      </c>
       <c r="G51" s="43">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" ref="G51:G58" si="13">E51*F51</f>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="40"/>
+      <c r="A52" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" s="12">
+        <v>5</v>
+      </c>
+      <c r="F52" s="40">
+        <v>13.19</v>
+      </c>
       <c r="G52" s="43">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>65.95</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3267,26 +3307,38 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G58" s="44">
-        <f>SUM(G3:G57)</f>
-        <v>14110.674000000003</v>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="43">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G59" s="44">
+        <f>SUM(G3:G58)</f>
+        <v>14178.424000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A50:G50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{A478C749-2080-B344-A289-CDF5D97B29A2}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{44C7BED6-AA93-3C43-B7CD-0009ABF6B6BB}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{B2AA866E-24F3-1646-ACED-D65EF9988155}"/>
-    <hyperlink ref="C39" r:id="rId4" xr:uid="{5010F871-A4EB-C348-B9FA-9AFAB7A4795F}"/>
+    <hyperlink ref="C40" r:id="rId4" xr:uid="{5010F871-A4EB-C348-B9FA-9AFAB7A4795F}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{6D0F970B-33A6-5741-B59A-13BE191765B5}"/>
-    <hyperlink ref="C45" r:id="rId6" xr:uid="{6E9AF94B-6606-EF47-BF3F-E19A5CFAFBEA}"/>
+    <hyperlink ref="C46" r:id="rId6" xr:uid="{6E9AF94B-6606-EF47-BF3F-E19A5CFAFBEA}"/>
     <hyperlink ref="C7" r:id="rId7" xr:uid="{D08990E8-0BCD-A44E-8FA8-5BE704D9FBEC}"/>
     <hyperlink ref="C8" r:id="rId8" xr:uid="{E2E6BF14-5F83-F745-A590-905519EB4A90}"/>
     <hyperlink ref="C9" r:id="rId9" xr:uid="{53620724-76B4-204B-AE5B-48ED373D3F0E}"/>
@@ -3296,33 +3348,34 @@
     <hyperlink ref="C18" r:id="rId13" xr:uid="{0D761B1C-BFCE-CA4C-AC56-8959BBCD1D8C}"/>
     <hyperlink ref="C13" r:id="rId14" xr:uid="{C2BA66AB-51D1-4E48-BDF6-5786EE1F2757}"/>
     <hyperlink ref="C11" r:id="rId15" xr:uid="{5A619F16-5DF6-7A47-930C-607E13BD2744}"/>
-    <hyperlink ref="C19" r:id="rId16" xr:uid="{63E6DFF5-E6E6-9D48-BEF0-976C1610D4CA}"/>
+    <hyperlink ref="C20" r:id="rId16" xr:uid="{63E6DFF5-E6E6-9D48-BEF0-976C1610D4CA}"/>
     <hyperlink ref="C17" r:id="rId17" xr:uid="{33FB920F-0669-0043-8C0C-BC6FBFCB38E1}"/>
     <hyperlink ref="C14" r:id="rId18" xr:uid="{E3D98391-497D-E645-A06E-B9C450FAA734}"/>
     <hyperlink ref="C15" r:id="rId19" xr:uid="{A82B3F0C-F6F0-BA48-95E6-EDBA66CD97B8}"/>
-    <hyperlink ref="C32" r:id="rId20" xr:uid="{D95FFA29-399D-6745-AC54-EDBAF115DD55}"/>
-    <hyperlink ref="C34" r:id="rId21" xr:uid="{DE78C3B5-25F3-B54C-AF32-A45A3CCF82C6}"/>
-    <hyperlink ref="C24" r:id="rId22" xr:uid="{E5990545-4A5C-BF4D-A2E3-33113701B5BE}"/>
-    <hyperlink ref="C25" r:id="rId23" xr:uid="{D97E6BC1-9B0F-7E4B-8DD8-6831F4863D0B}"/>
-    <hyperlink ref="C36" r:id="rId24" xr:uid="{52B47181-A334-734F-89EA-4D3CC6EE8FEE}"/>
-    <hyperlink ref="C43" r:id="rId25" xr:uid="{9DED03EC-6FA0-E340-9F64-4A2AFDB1BB32}"/>
-    <hyperlink ref="C33" r:id="rId26" xr:uid="{1B940CD5-6B42-114A-91F4-C00313929BF7}"/>
-    <hyperlink ref="C35" r:id="rId27" xr:uid="{9BF33B54-D294-6A41-BBDB-50238FA80D2D}"/>
-    <hyperlink ref="C40" r:id="rId28" xr:uid="{5D41B570-A2D6-AF45-8AF9-F20A8D241585}"/>
-    <hyperlink ref="C41" r:id="rId29" xr:uid="{F14BE297-86D6-B04A-98BE-ECD2D9A15FD8}"/>
-    <hyperlink ref="C20" r:id="rId30" xr:uid="{A0566B4B-F7CD-C14A-9EBE-943CA43F653D}"/>
-    <hyperlink ref="C21" r:id="rId31" xr:uid="{4BBCC18B-64B9-3948-8B17-249473C5AF6C}"/>
-    <hyperlink ref="C47" r:id="rId32" xr:uid="{AFDE7C59-FB6E-0B4D-A90B-C615F01A2424}"/>
-    <hyperlink ref="C46" r:id="rId33" xr:uid="{7295D0B3-C7AB-5D42-9A78-48C8E9745CA1}"/>
-    <hyperlink ref="C48" r:id="rId34" xr:uid="{0CFFB14A-47E8-B945-BCEB-B671BA1D6F52}"/>
-    <hyperlink ref="C27" r:id="rId35" xr:uid="{6A187383-C123-564D-BC92-969FA3FB5726}"/>
-    <hyperlink ref="C23" r:id="rId36" xr:uid="{1A29D440-BF31-E94C-BCA6-0C1202A21991}"/>
-    <hyperlink ref="C28" r:id="rId37" xr:uid="{36344359-AB27-274E-A2FC-98CD85B6FB8C}"/>
-    <hyperlink ref="C29" r:id="rId38" xr:uid="{A971E1C7-2D55-DA4F-9835-BC42C1DB56AF}"/>
-    <hyperlink ref="C37" r:id="rId39" xr:uid="{902445E2-BD52-B240-B54D-20CF95DAB079}"/>
-    <hyperlink ref="C26" r:id="rId40" xr:uid="{D0310BD2-7368-3C4A-AB34-40C7279D4F0B}"/>
-    <hyperlink ref="C30" r:id="rId41" xr:uid="{FAD92DE1-A270-F24C-8E9F-F880408C8288}"/>
-    <hyperlink ref="C22" r:id="rId42" xr:uid="{3E7B7CBC-84DD-1241-A9BD-85A9EBC5992B}"/>
+    <hyperlink ref="C33" r:id="rId20" xr:uid="{D95FFA29-399D-6745-AC54-EDBAF115DD55}"/>
+    <hyperlink ref="C35" r:id="rId21" xr:uid="{DE78C3B5-25F3-B54C-AF32-A45A3CCF82C6}"/>
+    <hyperlink ref="C25" r:id="rId22" xr:uid="{E5990545-4A5C-BF4D-A2E3-33113701B5BE}"/>
+    <hyperlink ref="C26" r:id="rId23" xr:uid="{D97E6BC1-9B0F-7E4B-8DD8-6831F4863D0B}"/>
+    <hyperlink ref="C37" r:id="rId24" xr:uid="{52B47181-A334-734F-89EA-4D3CC6EE8FEE}"/>
+    <hyperlink ref="C44" r:id="rId25" xr:uid="{9DED03EC-6FA0-E340-9F64-4A2AFDB1BB32}"/>
+    <hyperlink ref="C34" r:id="rId26" xr:uid="{1B940CD5-6B42-114A-91F4-C00313929BF7}"/>
+    <hyperlink ref="C36" r:id="rId27" xr:uid="{9BF33B54-D294-6A41-BBDB-50238FA80D2D}"/>
+    <hyperlink ref="C41" r:id="rId28" xr:uid="{5D41B570-A2D6-AF45-8AF9-F20A8D241585}"/>
+    <hyperlink ref="C42" r:id="rId29" xr:uid="{F14BE297-86D6-B04A-98BE-ECD2D9A15FD8}"/>
+    <hyperlink ref="C21" r:id="rId30" xr:uid="{A0566B4B-F7CD-C14A-9EBE-943CA43F653D}"/>
+    <hyperlink ref="C22" r:id="rId31" xr:uid="{4BBCC18B-64B9-3948-8B17-249473C5AF6C}"/>
+    <hyperlink ref="C48" r:id="rId32" xr:uid="{AFDE7C59-FB6E-0B4D-A90B-C615F01A2424}"/>
+    <hyperlink ref="C47" r:id="rId33" xr:uid="{7295D0B3-C7AB-5D42-9A78-48C8E9745CA1}"/>
+    <hyperlink ref="C49" r:id="rId34" xr:uid="{0CFFB14A-47E8-B945-BCEB-B671BA1D6F52}"/>
+    <hyperlink ref="C28" r:id="rId35" xr:uid="{6A187383-C123-564D-BC92-969FA3FB5726}"/>
+    <hyperlink ref="C24" r:id="rId36" xr:uid="{1A29D440-BF31-E94C-BCA6-0C1202A21991}"/>
+    <hyperlink ref="C29" r:id="rId37" xr:uid="{36344359-AB27-274E-A2FC-98CD85B6FB8C}"/>
+    <hyperlink ref="C30" r:id="rId38" xr:uid="{A971E1C7-2D55-DA4F-9835-BC42C1DB56AF}"/>
+    <hyperlink ref="C38" r:id="rId39" xr:uid="{902445E2-BD52-B240-B54D-20CF95DAB079}"/>
+    <hyperlink ref="C27" r:id="rId40" xr:uid="{D0310BD2-7368-3C4A-AB34-40C7279D4F0B}"/>
+    <hyperlink ref="C31" r:id="rId41" xr:uid="{FAD92DE1-A270-F24C-8E9F-F880408C8288}"/>
+    <hyperlink ref="C23" r:id="rId42" xr:uid="{3E7B7CBC-84DD-1241-A9BD-85A9EBC5992B}"/>
+    <hyperlink ref="C52" r:id="rId43" xr:uid="{164D90D5-3E91-3245-93D1-4C111CB2C8F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>